<commit_message>
Fixed a bug in the model creation template.
</commit_message>
<xml_diff>
--- a/model creation template.xlsx
+++ b/model creation template.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B1AE54-EAEE-4F26-B8AF-2238066E661D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Data" sheetId="2" r:id="rId1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="190">
   <si>
     <t>column name</t>
   </si>
@@ -593,6 +594,15 @@
   </si>
   <si>
     <t>AsOfDate</t>
+  </si>
+  <si>
+    <t>Schema</t>
+  </si>
+  <si>
+    <t>dw</t>
+  </si>
+  <si>
+    <t>ExchangesCK</t>
   </si>
 </sst>
 </file>
@@ -2806,7 +2816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
@@ -2831,10 +2841,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2858,13 +2868,21 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -3191,121 +3209,131 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="4" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.5703125" customWidth="1"/>
-    <col min="6" max="6" width="156.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="87.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="155.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="5" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.5703125" customWidth="1"/>
+    <col min="7" max="7" width="156.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="87.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="155.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" t="s">
         <v>161</v>
-      </c>
-      <c r="B2" t="s">
-        <v>160</v>
       </c>
       <c r="C2" t="s">
         <v>160</v>
       </c>
-      <c r="D2" t="e">
-        <f>VLOOKUP(B2,'Dimension List'!A:C,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E2" t="e">
-        <f>D2</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F2" t="e">
-        <f>"ALTER TABLE [dbo].["&amp;A2&amp;"]  WITH CHECK ADD CONSTRAINT [FK_"&amp;A2&amp;"_"&amp;B2&amp;"] FOREIGN KEY(["&amp;D2&amp;"])"</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G2" t="e">
-        <f t="shared" ref="G2" si="0">"REFERENCES [dbo].["&amp;C2&amp;"] (["&amp;E2&amp;"])"</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H2" t="e">
-        <f t="shared" ref="H2" si="1">F2&amp;" "&amp;G2</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2" t="str">
+        <f>VLOOKUP(C2,'Dimension List'!A:C,3,FALSE)</f>
+        <v>ExchangesCK</v>
+      </c>
+      <c r="F2" t="str">
+        <f>E2</f>
+        <v>ExchangesCK</v>
+      </c>
+      <c r="G2" t="str">
+        <f>"ALTER TABLE ["&amp;A2&amp;"].["&amp;B2&amp;"]  WITH CHECK ADD CONSTRAINT [FK_"&amp;B2&amp;"_"&amp;C2&amp;"] FOREIGN KEY(["&amp;E2&amp;"])"</f>
+        <v>ALTER TABLE [dw].[FactExchangeCloseData]  WITH CHECK ADD CONSTRAINT [FK_FactExchangeCloseData_DimExchanges] FOREIGN KEY([ExchangesCK])</v>
+      </c>
+      <c r="H2" t="str">
+        <f>"REFERENCES ["&amp;A2&amp;"].["&amp;D2&amp;"] (["&amp;F2&amp;"])"</f>
+        <v>REFERENCES [dw].[DimExchanges] ([ExchangesCK])</v>
+      </c>
+      <c r="I2" t="str">
+        <f t="shared" ref="I2" si="0">G2&amp;" "&amp;H2</f>
+        <v>ALTER TABLE [dw].[FactExchangeCloseData]  WITH CHECK ADD CONSTRAINT [FK_FactExchangeCloseData_DimExchanges] FOREIGN KEY([ExchangesCK]) REFERENCES [dw].[DimExchanges] ([ExchangesCK])</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" t="s">
         <v>161</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>163</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>164</v>
       </c>
-      <c r="D3" t="e">
-        <f>VLOOKUP(B3,'Dimension List'!A:C,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="E3" t="str">
+        <f>VLOOKUP(C3,'Dimension List'!A:C,3,FALSE)</f>
+        <v>DateCK</v>
+      </c>
+      <c r="F3" t="s">
         <v>165</v>
       </c>
-      <c r="F3" t="e">
-        <f>"ALTER TABLE [dbo].["&amp;A3&amp;"]  WITH CHECK ADD CONSTRAINT [FK_"&amp;A3&amp;"_"&amp;B3&amp;"] FOREIGN KEY(["&amp;D3&amp;"])"</f>
-        <v>#N/A</v>
-      </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3" si="2">"REFERENCES [dbo].["&amp;C3&amp;"] (["&amp;E3&amp;"])"</f>
-        <v>REFERENCES [dbo].[DimDate] ([DateCK])</v>
-      </c>
-      <c r="H3" t="e">
-        <f t="shared" ref="H3" si="3">F3&amp;" "&amp;G3</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F22" t="s">
+        <f>"ALTER TABLE ["&amp;A3&amp;"].["&amp;B3&amp;"]  WITH CHECK ADD CONSTRAINT [FK_"&amp;B3&amp;"_"&amp;C3&amp;"] FOREIGN KEY(["&amp;E3&amp;"])"</f>
+        <v>ALTER TABLE [dw].[FactExchangeCloseData]  WITH CHECK ADD CONSTRAINT [FK_FactExchangeCloseData_DimLastTradeDateTime] FOREIGN KEY([DateCK])</v>
+      </c>
+      <c r="H3" t="str">
+        <f>"REFERENCES ["&amp;A3&amp;"].["&amp;D3&amp;"] (["&amp;F3&amp;"])"</f>
+        <v>REFERENCES [dw].[DimDate] ([DateCK])</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3" si="1">G3&amp;" "&amp;H3</f>
+        <v>ALTER TABLE [dw].[FactExchangeCloseData]  WITH CHECK ADD CONSTRAINT [FK_FactExchangeCloseData_DimLastTradeDateTime] FOREIGN KEY([DateCK]) REFERENCES [dw].[DimDate] ([DateCK])</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>